<commit_message>
Code cleaning and parallelism on
Also adding time into results
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -61,11 +61,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -431,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,13 +448,15 @@
     <col width="7.199999999999999" customWidth="1" min="1" max="1"/>
     <col width="15.6" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="14.4" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="18" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="39.6" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="18" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -456,822 +464,1137 @@
           <t>File Tested</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Run Status</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Time Completation (hh:mm:ss:ms)</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Error Message</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>40509</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr"/>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.103</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>ac0</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr"/>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>ac1</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr"/>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" s="4" t="inlineStr">
         <is>
           <t>ac2</t>
         </is>
       </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr"/>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>ac3</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr"/>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="4" t="inlineStr">
         <is>
           <t>ac4</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="inlineStr"/>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>ac5</t>
         </is>
       </c>
-      <c r="C9" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D9" s="3" t="inlineStr"/>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>ac6</t>
         </is>
       </c>
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="inlineStr"/>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E10" s="5" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>ac7</t>
         </is>
       </c>
-      <c r="C11" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="inlineStr"/>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" s="4" t="inlineStr">
         <is>
           <t>ac8</t>
         </is>
       </c>
-      <c r="C12" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="inlineStr"/>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B13" s="4" t="inlineStr">
         <is>
           <t>ac9</t>
         </is>
       </c>
-      <c r="C13" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D13" s="3" t="inlineStr"/>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="4" t="inlineStr">
         <is>
           <t>ac10</t>
         </is>
       </c>
-      <c r="C14" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr"/>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" s="4" t="inlineStr">
         <is>
           <t>ac11</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr"/>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" s="4" t="inlineStr">
         <is>
           <t>ac12</t>
         </is>
       </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr"/>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E16" s="5" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" s="4" t="inlineStr">
         <is>
           <t>ac13</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr"/>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E17" s="5" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B18" s="4" t="inlineStr">
         <is>
           <t>ac14</t>
         </is>
       </c>
-      <c r="C18" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D18" s="3" t="inlineStr"/>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E18" s="5" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B19" s="4" t="inlineStr">
         <is>
           <t>ac15</t>
         </is>
       </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="inlineStr"/>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E19" s="5" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="B20" s="3" t="inlineStr">
+      <c r="B20" s="4" t="inlineStr">
         <is>
           <t>ac16</t>
         </is>
       </c>
-      <c r="C20" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="inlineStr"/>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E20" s="5" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" s="4" t="inlineStr">
         <is>
           <t>ac17</t>
         </is>
       </c>
-      <c r="C21" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D21" s="3" t="inlineStr"/>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B22" s="4" t="inlineStr">
         <is>
           <t>ac18</t>
         </is>
       </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="inlineStr"/>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B23" s="4" t="inlineStr">
         <is>
           <t>ac19</t>
         </is>
       </c>
-      <c r="C23" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D23" s="3" t="inlineStr"/>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B24" s="4" t="inlineStr">
         <is>
           <t>ac20</t>
         </is>
       </c>
-      <c r="C24" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D24" s="3" t="inlineStr"/>
+      <c r="C24" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="B25" s="3" t="inlineStr">
+      <c r="B25" s="4" t="inlineStr">
         <is>
           <t>cr0</t>
         </is>
       </c>
-      <c r="C25" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D25" s="3" t="inlineStr"/>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="B26" s="3" t="inlineStr">
+      <c r="B26" s="4" t="inlineStr">
         <is>
           <t>cr1</t>
         </is>
       </c>
-      <c r="C26" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D26" s="3" t="inlineStr"/>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="B27" s="3" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>cr2</t>
         </is>
       </c>
-      <c r="C27" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D27" s="3" t="inlineStr"/>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="B28" s="3" t="inlineStr">
+      <c r="B28" s="4" t="inlineStr">
         <is>
           <t>cr3</t>
         </is>
       </c>
-      <c r="C28" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D28" s="3" t="inlineStr"/>
+      <c r="C28" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.015</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="B29" s="3" t="inlineStr">
+      <c r="B29" s="4" t="inlineStr">
         <is>
           <t>cr4</t>
         </is>
       </c>
-      <c r="C29" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D29" s="3" t="inlineStr"/>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="B30" s="3" t="inlineStr">
+      <c r="B30" s="4" t="inlineStr">
         <is>
           <t>cr5</t>
         </is>
       </c>
-      <c r="C30" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D30" s="3" t="inlineStr"/>
+      <c r="C30" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E30" s="5" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="B31" s="3" t="inlineStr">
+      <c r="B31" s="4" t="inlineStr">
         <is>
           <t>cr6</t>
         </is>
       </c>
-      <c r="C31" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="inlineStr"/>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="B32" s="3" t="inlineStr">
+      <c r="B32" s="4" t="inlineStr">
         <is>
           <t>cr7</t>
         </is>
       </c>
-      <c r="C32" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D32" s="3" t="inlineStr"/>
+      <c r="C32" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E32" s="5" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="B33" s="3" t="inlineStr">
+      <c r="B33" s="4" t="inlineStr">
         <is>
           <t>cr8</t>
         </is>
       </c>
-      <c r="C33" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D33" s="3" t="inlineStr"/>
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D33" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E33" s="5" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="B34" s="3" t="inlineStr">
+      <c r="B34" s="4" t="inlineStr">
         <is>
           <t>cr9</t>
         </is>
       </c>
-      <c r="C34" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D34" s="3" t="inlineStr"/>
+      <c r="C34" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D34" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E34" s="5" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="B35" s="3" t="inlineStr">
+      <c r="B35" s="4" t="inlineStr">
         <is>
           <t>cr10</t>
         </is>
       </c>
-      <c r="C35" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D35" s="3" t="inlineStr"/>
+      <c r="C35" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D35" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E35" s="5" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="B36" s="3" t="inlineStr">
+      <c r="B36" s="4" t="inlineStr">
         <is>
           <t>cr11</t>
         </is>
       </c>
-      <c r="C36" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D36" s="3" t="inlineStr"/>
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D36" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E36" s="5" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="B37" s="3" t="inlineStr">
+      <c r="B37" s="4" t="inlineStr">
         <is>
           <t>cr12</t>
         </is>
       </c>
-      <c r="C37" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D37" s="3" t="inlineStr"/>
+      <c r="C37" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D37" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E37" s="5" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="B38" s="3" t="inlineStr">
+      <c r="B38" s="4" t="inlineStr">
         <is>
           <t>cr13</t>
         </is>
       </c>
-      <c r="C38" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D38" s="3" t="inlineStr"/>
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D38" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E38" s="5" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="B39" s="3" t="inlineStr">
+      <c r="B39" s="4" t="inlineStr">
         <is>
           <t>sc0</t>
         </is>
       </c>
-      <c r="C39" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D39" s="3" t="inlineStr"/>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D39" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E39" s="5" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="B40" s="3" t="inlineStr">
+      <c r="B40" s="4" t="inlineStr">
         <is>
           <t>sc1</t>
         </is>
       </c>
-      <c r="C40" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D40" s="3" t="inlineStr"/>
+      <c r="C40" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D40" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E40" s="5" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="B41" s="3" t="inlineStr">
+      <c r="B41" s="4" t="inlineStr">
         <is>
           <t>sc2</t>
         </is>
       </c>
-      <c r="C41" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="inlineStr"/>
+      <c r="C41" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D41" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E41" s="5" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="B42" s="3" t="inlineStr">
+      <c r="B42" s="4" t="inlineStr">
         <is>
           <t>sc3</t>
         </is>
       </c>
-      <c r="C42" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D42" s="3" t="inlineStr"/>
+      <c r="C42" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D42" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E42" s="5" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="B43" s="3" t="inlineStr">
+      <c r="B43" s="4" t="inlineStr">
         <is>
           <t>sc4</t>
         </is>
       </c>
-      <c r="C43" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D43" s="3" t="inlineStr"/>
+      <c r="C43" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D43" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E43" s="5" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="B44" s="3" t="inlineStr">
+      <c r="B44" s="4" t="inlineStr">
         <is>
           <t>sc5</t>
         </is>
       </c>
-      <c r="C44" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="inlineStr"/>
+      <c r="C44" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D44" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E44" s="5" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="B45" s="3" t="inlineStr">
+      <c r="B45" s="4" t="inlineStr">
         <is>
           <t>sc6</t>
         </is>
       </c>
-      <c r="C45" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="inlineStr"/>
+      <c r="C45" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D45" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E45" s="5" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="B46" s="3" t="inlineStr">
+      <c r="B46" s="4" t="inlineStr">
         <is>
           <t>sc7</t>
         </is>
       </c>
-      <c r="C46" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="inlineStr"/>
+      <c r="C46" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D46" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E46" s="5" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="B47" s="3" t="inlineStr">
+      <c r="B47" s="4" t="inlineStr">
         <is>
           <t>sc8</t>
         </is>
       </c>
-      <c r="C47" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D47" s="3" t="inlineStr"/>
+      <c r="C47" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D47" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E47" s="5" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="B48" s="3" t="inlineStr">
+      <c r="B48" s="4" t="inlineStr">
         <is>
           <t>sc9</t>
         </is>
       </c>
-      <c r="C48" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="inlineStr"/>
+      <c r="C48" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D48" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E48" s="5" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="B49" s="3" t="inlineStr">
+      <c r="B49" s="4" t="inlineStr">
         <is>
           <t>sc10</t>
         </is>
       </c>
-      <c r="C49" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="inlineStr"/>
+      <c r="C49" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D49" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E49" s="5" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="B50" s="3" t="inlineStr">
+      <c r="B50" s="4" t="inlineStr">
         <is>
           <t>sc11</t>
         </is>
       </c>
-      <c r="C50" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="inlineStr"/>
+      <c r="C50" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D50" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E50" s="5" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="B51" s="3" t="inlineStr">
+      <c r="B51" s="4" t="inlineStr">
         <is>
           <t>sc12</t>
         </is>
       </c>
-      <c r="C51" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="inlineStr"/>
+      <c r="C51" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D51" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E51" s="5" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="B52" s="3" t="inlineStr">
+      <c r="B52" s="4" t="inlineStr">
         <is>
           <t>sc13</t>
         </is>
       </c>
-      <c r="C52" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D52" s="3" t="inlineStr"/>
+      <c r="C52" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D52" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E52" s="5" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="B53" s="3" t="inlineStr">
+      <c r="B53" s="4" t="inlineStr">
         <is>
           <t>three_cubes</t>
         </is>
       </c>
-      <c r="C53" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="inlineStr"/>
+      <c r="C53" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D53" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.018</t>
+        </is>
+      </c>
+      <c r="E53" s="5" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="B54" s="3" t="inlineStr">
+      <c r="B54" s="4" t="inlineStr">
         <is>
           <t>ttt0</t>
         </is>
       </c>
-      <c r="C54" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D54" s="3" t="inlineStr"/>
+      <c r="C54" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D54" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E54" s="5" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="B55" s="3" t="inlineStr">
+      <c r="B55" s="4" t="inlineStr">
         <is>
           <t>ttt1</t>
         </is>
       </c>
-      <c r="C55" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D55" s="3" t="inlineStr"/>
+      <c r="C55" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D55" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E55" s="5" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="B56" s="3" t="inlineStr">
+      <c r="B56" s="4" t="inlineStr">
         <is>
           <t>ttt2</t>
         </is>
       </c>
-      <c r="C56" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="inlineStr"/>
+      <c r="C56" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D56" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E56" s="5" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="B57" s="3" t="inlineStr">
+      <c r="B57" s="4" t="inlineStr">
         <is>
           <t>ttt3</t>
         </is>
       </c>
-      <c r="C57" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="inlineStr"/>
+      <c r="C57" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D57" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.014</t>
+        </is>
+      </c>
+      <c r="E57" s="5" t="inlineStr"/>
     </row>
     <row r="58">
-      <c r="B58" s="3" t="inlineStr">
+      <c r="B58" s="4" t="inlineStr">
         <is>
           <t>ttt4</t>
         </is>
       </c>
-      <c r="C58" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D58" s="3" t="inlineStr"/>
+      <c r="C58" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D58" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E58" s="5" t="inlineStr"/>
     </row>
     <row r="59">
-      <c r="B59" s="3" t="inlineStr">
+      <c r="B59" s="4" t="inlineStr">
         <is>
           <t>ttt5</t>
         </is>
       </c>
-      <c r="C59" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="inlineStr"/>
+      <c r="C59" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D59" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E59" s="5" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="B60" s="3" t="inlineStr">
+      <c r="B60" s="4" t="inlineStr">
         <is>
           <t>two_spheres</t>
         </is>
       </c>
-      <c r="C60" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D60" s="3" t="inlineStr"/>
+      <c r="C60" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D60" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.022</t>
+        </is>
+      </c>
+      <c r="E60" s="5" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="B61" s="3" t="inlineStr">
+      <c r="B61" s="4" t="inlineStr">
         <is>
           <t>vot0</t>
         </is>
       </c>
-      <c r="C61" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="inlineStr"/>
+      <c r="C61" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D61" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E61" s="5" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="B62" s="3" t="inlineStr">
+      <c r="B62" s="4" t="inlineStr">
         <is>
           <t>vot1</t>
         </is>
       </c>
-      <c r="C62" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D62" s="3" t="inlineStr"/>
+      <c r="C62" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D62" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E62" s="5" t="inlineStr"/>
     </row>
     <row r="63">
-      <c r="B63" s="3" t="inlineStr">
+      <c r="B63" s="4" t="inlineStr">
         <is>
           <t>vot2</t>
         </is>
       </c>
-      <c r="C63" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D63" s="3" t="inlineStr"/>
+      <c r="C63" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D63" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E63" s="5" t="inlineStr"/>
     </row>
     <row r="64">
-      <c r="B64" s="3" t="inlineStr">
+      <c r="B64" s="4" t="inlineStr">
         <is>
           <t>vot3</t>
         </is>
       </c>
-      <c r="C64" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D64" s="3" t="inlineStr"/>
+      <c r="C64" s="5" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="D64" s="5" t="inlineStr">
+        <is>
+          <t>00:00:00.013</t>
+        </is>
+      </c>
+      <c r="E64" s="5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
formatting and final test results
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.116</t>
+          <t>00:00:00:114</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr"/>
@@ -529,7 +529,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr"/>
@@ -547,7 +547,7 @@
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.014</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr"/>
@@ -583,7 +583,7 @@
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E8" s="5" t="inlineStr"/>
@@ -601,7 +601,7 @@
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E9" s="5" t="inlineStr"/>
@@ -619,7 +619,7 @@
       </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E10" s="5" t="inlineStr"/>
@@ -637,7 +637,7 @@
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E11" s="5" t="inlineStr"/>
@@ -655,7 +655,7 @@
       </c>
       <c r="D12" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E12" s="5" t="inlineStr"/>
@@ -673,7 +673,7 @@
       </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E13" s="5" t="inlineStr"/>
@@ -691,7 +691,7 @@
       </c>
       <c r="D14" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E14" s="5" t="inlineStr"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E15" s="5" t="inlineStr"/>
@@ -727,7 +727,7 @@
       </c>
       <c r="D16" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E16" s="5" t="inlineStr"/>
@@ -745,7 +745,7 @@
       </c>
       <c r="D17" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E17" s="5" t="inlineStr"/>
@@ -763,7 +763,7 @@
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr"/>
@@ -781,7 +781,7 @@
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.014</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E19" s="5" t="inlineStr"/>
@@ -799,7 +799,7 @@
       </c>
       <c r="D20" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E20" s="5" t="inlineStr"/>
@@ -817,7 +817,7 @@
       </c>
       <c r="D21" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E21" s="5" t="inlineStr"/>
@@ -835,7 +835,7 @@
       </c>
       <c r="D22" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E22" s="5" t="inlineStr"/>
@@ -853,7 +853,7 @@
       </c>
       <c r="D23" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.014</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E23" s="5" t="inlineStr"/>
@@ -871,7 +871,7 @@
       </c>
       <c r="D24" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E24" s="5" t="inlineStr"/>
@@ -889,7 +889,7 @@
       </c>
       <c r="D25" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E25" s="5" t="inlineStr"/>
@@ -907,7 +907,7 @@
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.015</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr"/>
@@ -943,7 +943,7 @@
       </c>
       <c r="D28" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E28" s="5" t="inlineStr"/>
@@ -961,7 +961,7 @@
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr"/>
@@ -979,7 +979,7 @@
       </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E30" s="5" t="inlineStr"/>
@@ -997,7 +997,7 @@
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.012</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E31" s="5" t="inlineStr"/>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D32" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E32" s="5" t="inlineStr"/>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="D33" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E33" s="5" t="inlineStr"/>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D34" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E34" s="5" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="D35" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:016</t>
         </is>
       </c>
       <c r="E35" s="5" t="inlineStr"/>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D36" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.016</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E36" s="5" t="inlineStr"/>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="D37" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.012</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E37" s="5" t="inlineStr"/>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="D38" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E38" s="5" t="inlineStr"/>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D39" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E39" s="5" t="inlineStr"/>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="D40" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E40" s="5" t="inlineStr"/>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D41" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.012</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E41" s="5" t="inlineStr"/>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D42" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.012</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E42" s="5" t="inlineStr"/>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="D43" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.012</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E43" s="5" t="inlineStr"/>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D44" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E44" s="5" t="inlineStr"/>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D45" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.012</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E45" s="5" t="inlineStr"/>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D46" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E46" s="5" t="inlineStr"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D47" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E47" s="5" t="inlineStr"/>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="D48" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E48" s="5" t="inlineStr"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="D49" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E49" s="5" t="inlineStr"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="D50" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:012</t>
         </is>
       </c>
       <c r="E50" s="5" t="inlineStr"/>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="D51" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.014</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E51" s="5" t="inlineStr"/>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D52" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E52" s="5" t="inlineStr"/>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="D53" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.018</t>
+          <t>00:00:00:017</t>
         </is>
       </c>
       <c r="E53" s="5" t="inlineStr"/>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="D54" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.014</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E54" s="5" t="inlineStr"/>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="D55" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E55" s="5" t="inlineStr"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D56" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E56" s="5" t="inlineStr"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D57" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.014</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E57" s="5" t="inlineStr"/>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="D58" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.014</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E58" s="5" t="inlineStr"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="D59" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E59" s="5" t="inlineStr"/>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="D60" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.022</t>
+          <t>00:00:00:025</t>
         </is>
       </c>
       <c r="E60" s="5" t="inlineStr"/>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="D61" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E61" s="5" t="inlineStr"/>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="D62" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E62" s="5" t="inlineStr"/>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D63" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E63" s="5" t="inlineStr"/>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="D64" s="5" t="inlineStr">
         <is>
-          <t>00:00:00.013</t>
+          <t>00:00:00:013</t>
         </is>
       </c>
       <c r="E64" s="5" t="inlineStr"/>

</xml_diff>

<commit_message>
cleaning #1 before pull request
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="7.199999999999999" customWidth="1" min="1" max="1"/>
-    <col width="15.6" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="18" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="14.4" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="39.6" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="18" bestFit="1" customWidth="1" min="5" max="5"/>
@@ -483,7 +483,7 @@
     <row r="3">
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>32770</t>
+          <t>40509</t>
         </is>
       </c>
       <c r="C3" s="5" t="inlineStr">
@@ -493,7 +493,7 @@
       </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:324</t>
+          <t>00:00:00:087</t>
         </is>
       </c>
       <c r="E3" s="5" t="inlineStr"/>
@@ -501,7 +501,7 @@
     <row r="4">
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>34783</t>
+          <t>ac0</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:124</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E4" s="5" t="inlineStr"/>
@@ -519,7 +519,7 @@
     <row r="5">
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>34784</t>
+          <t>ac1</t>
         </is>
       </c>
       <c r="C5" s="5" t="inlineStr">
@@ -529,7 +529,7 @@
       </c>
       <c r="D5" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:137</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E5" s="5" t="inlineStr"/>
@@ -537,7 +537,7 @@
     <row r="6">
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>34785</t>
+          <t>ac2</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:051</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr"/>
@@ -555,7 +555,7 @@
     <row r="7">
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>35269</t>
+          <t>ac3</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:158</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr"/>
@@ -573,7 +573,7 @@
     <row r="8">
       <c r="B8" s="4" t="inlineStr">
         <is>
-          <t>36069</t>
+          <t>ac4</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:011</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E8" s="5" t="inlineStr"/>
@@ -591,7 +591,7 @@
     <row r="9">
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>36075</t>
+          <t>ac5</t>
         </is>
       </c>
       <c r="C9" s="5" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:011</t>
+          <t>00:00:00:009</t>
         </is>
       </c>
       <c r="E9" s="5" t="inlineStr"/>
@@ -609,7 +609,7 @@
     <row r="10">
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>36082</t>
+          <t>ac6</t>
         </is>
       </c>
       <c r="C10" s="5" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:011</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E10" s="5" t="inlineStr"/>
@@ -627,7 +627,7 @@
     <row r="11">
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>36086</t>
+          <t>ac7</t>
         </is>
       </c>
       <c r="C11" s="5" t="inlineStr">
@@ -637,7 +637,7 @@
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:013</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E11" s="5" t="inlineStr"/>
@@ -645,7 +645,7 @@
     <row r="12">
       <c r="B12" s="4" t="inlineStr">
         <is>
-          <t>36088</t>
+          <t>ac8</t>
         </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
@@ -655,7 +655,7 @@
       </c>
       <c r="D12" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:225</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E12" s="5" t="inlineStr"/>
@@ -663,7 +663,7 @@
     <row r="13">
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>36090</t>
+          <t>ac9</t>
         </is>
       </c>
       <c r="C13" s="5" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:013</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E13" s="5" t="inlineStr"/>
@@ -681,7 +681,7 @@
     <row r="14">
       <c r="B14" s="4" t="inlineStr">
         <is>
-          <t>36091</t>
+          <t>ac10</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
@@ -691,7 +691,7 @@
       </c>
       <c r="D14" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:100</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E14" s="5" t="inlineStr"/>
@@ -699,7 +699,7 @@
     <row r="15">
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>36092</t>
+          <t>ac11</t>
         </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
@@ -709,7 +709,7 @@
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:123</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E15" s="5" t="inlineStr"/>
@@ -717,7 +717,7 @@
     <row r="16">
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>36371</t>
+          <t>ac12</t>
         </is>
       </c>
       <c r="C16" s="5" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="D16" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:173</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E16" s="5" t="inlineStr"/>
@@ -735,7 +735,7 @@
     <row r="17">
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>36372</t>
+          <t>ac13</t>
         </is>
       </c>
       <c r="C17" s="5" t="inlineStr">
@@ -745,7 +745,7 @@
       </c>
       <c r="D17" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:010</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E17" s="5" t="inlineStr"/>
@@ -753,7 +753,7 @@
     <row r="18">
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>36373</t>
+          <t>ac14</t>
         </is>
       </c>
       <c r="C18" s="5" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:013</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr"/>
@@ -771,7 +771,7 @@
     <row r="19">
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>36374</t>
+          <t>ac15</t>
         </is>
       </c>
       <c r="C19" s="5" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:207</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E19" s="5" t="inlineStr"/>
@@ -789,7 +789,7 @@
     <row r="20">
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>37003</t>
+          <t>ac16</t>
         </is>
       </c>
       <c r="C20" s="5" t="inlineStr">
@@ -799,7 +799,7 @@
       </c>
       <c r="D20" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:458</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E20" s="5" t="inlineStr"/>
@@ -807,7 +807,7 @@
     <row r="21">
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>37004</t>
+          <t>ac17</t>
         </is>
       </c>
       <c r="C21" s="5" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="D21" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:158</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E21" s="5" t="inlineStr"/>
@@ -825,7 +825,7 @@
     <row r="22">
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>37009</t>
+          <t>ac18</t>
         </is>
       </c>
       <c r="C22" s="5" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="D22" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:118</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E22" s="5" t="inlineStr"/>
@@ -843,7 +843,7 @@
     <row r="23">
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>37010</t>
+          <t>ac19</t>
         </is>
       </c>
       <c r="C23" s="5" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="D23" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:060</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E23" s="5" t="inlineStr"/>
@@ -861,7 +861,7 @@
     <row r="24">
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>37011</t>
+          <t>ac20</t>
         </is>
       </c>
       <c r="C24" s="5" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D24" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:097</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E24" s="5" t="inlineStr"/>
@@ -879,7 +879,7 @@
     <row r="25">
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>37012</t>
+          <t>cr0</t>
         </is>
       </c>
       <c r="C25" s="5" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="D25" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:015</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E25" s="5" t="inlineStr"/>
@@ -897,7 +897,7 @@
     <row r="26">
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>37065</t>
+          <t>cr1</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:016</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr"/>
@@ -915,7 +915,7 @@
     <row r="27">
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>37091</t>
+          <t>cr2</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:010</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr"/>
@@ -933,7 +933,7 @@
     <row r="28">
       <c r="B28" s="4" t="inlineStr">
         <is>
-          <t>37093</t>
+          <t>cr3</t>
         </is>
       </c>
       <c r="C28" s="5" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="D28" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:013</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E28" s="5" t="inlineStr"/>
@@ -951,7 +951,7 @@
     <row r="29">
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>37095</t>
+          <t>cr4</t>
         </is>
       </c>
       <c r="C29" s="5" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:014</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E29" s="5" t="inlineStr"/>
@@ -969,7 +969,7 @@
     <row r="30">
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>37111</t>
+          <t>cr5</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:412</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E30" s="5" t="inlineStr"/>
@@ -987,7 +987,7 @@
     <row r="31">
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>37137</t>
+          <t>cr6</t>
         </is>
       </c>
       <c r="C31" s="5" t="inlineStr">
@@ -997,7 +997,7 @@
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:322</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E31" s="5" t="inlineStr"/>
@@ -1005,7 +1005,7 @@
     <row r="32">
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>37179</t>
+          <t>cr7</t>
         </is>
       </c>
       <c r="C32" s="5" t="inlineStr">
@@ -1015,7 +1015,7 @@
       </c>
       <c r="D32" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:015</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E32" s="5" t="inlineStr"/>
@@ -1023,7 +1023,7 @@
     <row r="33">
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>37211</t>
+          <t>cr8</t>
         </is>
       </c>
       <c r="C33" s="5" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="D33" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:022</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E33" s="5" t="inlineStr"/>
@@ -1041,7 +1041,7 @@
     <row r="34">
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>37213</t>
+          <t>cr9</t>
         </is>
       </c>
       <c r="C34" s="5" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="D34" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:023</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E34" s="5" t="inlineStr"/>
@@ -1059,7 +1059,7 @@
     <row r="35">
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>37215</t>
+          <t>cr10</t>
         </is>
       </c>
       <c r="C35" s="5" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="D35" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:036</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E35" s="5" t="inlineStr"/>
@@ -1077,7 +1077,7 @@
     <row r="36">
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>37217</t>
+          <t>cr11</t>
         </is>
       </c>
       <c r="C36" s="5" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="D36" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:017</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E36" s="5" t="inlineStr"/>
@@ -1095,7 +1095,7 @@
     <row r="37">
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>37219</t>
+          <t>cr12</t>
         </is>
       </c>
       <c r="C37" s="5" t="inlineStr">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="D37" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:027</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E37" s="5" t="inlineStr"/>
@@ -1113,7 +1113,7 @@
     <row r="38">
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>37221</t>
+          <t>cr13</t>
         </is>
       </c>
       <c r="C38" s="5" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="D38" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:015</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E38" s="5" t="inlineStr"/>
@@ -1131,7 +1131,7 @@
     <row r="39">
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>37223</t>
+          <t>sc0</t>
         </is>
       </c>
       <c r="C39" s="5" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D39" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:031</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E39" s="5" t="inlineStr"/>
@@ -1149,7 +1149,7 @@
     <row r="40">
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>37225</t>
+          <t>sc1</t>
         </is>
       </c>
       <c r="C40" s="5" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="D40" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:014</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E40" s="5" t="inlineStr"/>
@@ -1167,7 +1167,7 @@
     <row r="41">
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>37227</t>
+          <t>sc2</t>
         </is>
       </c>
       <c r="C41" s="5" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D41" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:027</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E41" s="5" t="inlineStr"/>
@@ -1185,7 +1185,7 @@
     <row r="42">
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>37229</t>
+          <t>sc3</t>
         </is>
       </c>
       <c r="C42" s="5" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D42" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:018</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E42" s="5" t="inlineStr"/>
@@ -1203,7 +1203,7 @@
     <row r="43">
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>37266</t>
+          <t>sc4</t>
         </is>
       </c>
       <c r="C43" s="5" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="D43" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:132</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E43" s="5" t="inlineStr"/>
@@ -1221,7 +1221,7 @@
     <row r="44">
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>37267</t>
+          <t>sc5</t>
         </is>
       </c>
       <c r="C44" s="5" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D44" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:186</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E44" s="5" t="inlineStr"/>
@@ -1239,7 +1239,7 @@
     <row r="45">
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>37272</t>
+          <t>sc6</t>
         </is>
       </c>
       <c r="C45" s="5" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="D45" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:029</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E45" s="5" t="inlineStr"/>
@@ -1257,7 +1257,7 @@
     <row r="46">
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>37274</t>
+          <t>sc7</t>
         </is>
       </c>
       <c r="C46" s="5" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D46" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:016</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E46" s="5" t="inlineStr"/>
@@ -1275,7 +1275,7 @@
     <row r="47">
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>37275</t>
+          <t>sc8</t>
         </is>
       </c>
       <c r="C47" s="5" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D47" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:106</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E47" s="5" t="inlineStr"/>
@@ -1293,7 +1293,7 @@
     <row r="48">
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>37276</t>
+          <t>sc9</t>
         </is>
       </c>
       <c r="C48" s="5" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="D48" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:019</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E48" s="5" t="inlineStr"/>
@@ -1311,7 +1311,7 @@
     <row r="49">
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>37278</t>
+          <t>sc10</t>
         </is>
       </c>
       <c r="C49" s="5" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="D49" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:018</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E49" s="5" t="inlineStr"/>
@@ -1329,7 +1329,7 @@
     <row r="50">
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>37280</t>
+          <t>sc11</t>
         </is>
       </c>
       <c r="C50" s="5" t="inlineStr">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="D50" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:018</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E50" s="5" t="inlineStr"/>
@@ -1347,7 +1347,7 @@
     <row r="51">
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>37282</t>
+          <t>sc12</t>
         </is>
       </c>
       <c r="C51" s="5" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="D51" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:030</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E51" s="5" t="inlineStr"/>
@@ -1365,7 +1365,7 @@
     <row r="52">
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>37283</t>
+          <t>sc13</t>
         </is>
       </c>
       <c r="C52" s="5" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D52" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:016</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E52" s="5" t="inlineStr"/>
@@ -1383,7 +1383,7 @@
     <row r="53">
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>37284</t>
+          <t>test_point_1</t>
         </is>
       </c>
       <c r="C53" s="5" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="D53" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:053</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E53" s="5" t="inlineStr"/>
@@ -1401,7 +1401,7 @@
     <row r="54">
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>37285</t>
+          <t>test_point_e3</t>
         </is>
       </c>
       <c r="C54" s="5" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="D54" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:013</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E54" s="5" t="inlineStr"/>
@@ -1419,7 +1419,7 @@
     <row r="55">
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>37286</t>
+          <t>three_cubes</t>
         </is>
       </c>
       <c r="C55" s="5" t="inlineStr">
@@ -1429,7 +1429,7 @@
       </c>
       <c r="D55" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:019</t>
+          <t>00:00:00:009</t>
         </is>
       </c>
       <c r="E55" s="5" t="inlineStr"/>
@@ -1437,7 +1437,7 @@
     <row r="56">
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>37287</t>
+          <t>ttt0</t>
         </is>
       </c>
       <c r="C56" s="5" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="D56" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:017</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E56" s="5" t="inlineStr"/>
@@ -1455,7 +1455,7 @@
     <row r="57">
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>37288</t>
+          <t>ttt1</t>
         </is>
       </c>
       <c r="C57" s="5" t="inlineStr">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D57" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:026</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E57" s="5" t="inlineStr"/>
@@ -1473,7 +1473,7 @@
     <row r="58">
       <c r="B58" s="4" t="inlineStr">
         <is>
-          <t>37289</t>
+          <t>ttt2</t>
         </is>
       </c>
       <c r="C58" s="5" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="D58" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:035</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E58" s="5" t="inlineStr"/>
@@ -1491,7 +1491,7 @@
     <row r="59">
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>37303</t>
+          <t>ttt3</t>
         </is>
       </c>
       <c r="C59" s="5" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="D59" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:013</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E59" s="5" t="inlineStr"/>
@@ -1509,7 +1509,7 @@
     <row r="60">
       <c r="B60" s="4" t="inlineStr">
         <is>
-          <t>37304</t>
+          <t>ttt4</t>
         </is>
       </c>
       <c r="C60" s="5" t="inlineStr">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="D60" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:064</t>
+          <t>00:00:00:007</t>
         </is>
       </c>
       <c r="E60" s="5" t="inlineStr"/>
@@ -1527,7 +1527,7 @@
     <row r="61">
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>37322</t>
+          <t>ttt5</t>
         </is>
       </c>
       <c r="C61" s="5" t="inlineStr">
@@ -1545,7 +1545,7 @@
     <row r="62">
       <c r="B62" s="4" t="inlineStr">
         <is>
-          <t>37323</t>
+          <t>two_spheres</t>
         </is>
       </c>
       <c r="C62" s="5" t="inlineStr">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="D62" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:013</t>
+          <t>00:00:00:016</t>
         </is>
       </c>
       <c r="E62" s="5" t="inlineStr"/>
@@ -1563,7 +1563,7 @@
     <row r="63">
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>37325</t>
+          <t>vot0</t>
         </is>
       </c>
       <c r="C63" s="5" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D63" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:014</t>
+          <t>00:00:00:010</t>
         </is>
       </c>
       <c r="E63" s="5" t="inlineStr"/>
@@ -1581,7 +1581,7 @@
     <row r="64">
       <c r="B64" s="4" t="inlineStr">
         <is>
-          <t>37326</t>
+          <t>vot1</t>
         </is>
       </c>
       <c r="C64" s="5" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="D64" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:018</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E64" s="5" t="inlineStr"/>
@@ -1599,7 +1599,7 @@
     <row r="65">
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>37327</t>
+          <t>vot2</t>
         </is>
       </c>
       <c r="C65" s="5" t="inlineStr">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="D65" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:019</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E65" s="5" t="inlineStr"/>
@@ -1617,7 +1617,7 @@
     <row r="66">
       <c r="B66" s="4" t="inlineStr">
         <is>
-          <t>37328</t>
+          <t>vot3</t>
         </is>
       </c>
       <c r="C66" s="5" t="inlineStr">
@@ -1627,406 +1627,10 @@
       </c>
       <c r="D66" s="5" t="inlineStr">
         <is>
-          <t>00:00:00:023</t>
+          <t>00:00:00:008</t>
         </is>
       </c>
       <c r="E66" s="5" t="inlineStr"/>
-    </row>
-    <row r="67">
-      <c r="B67" s="4" t="inlineStr">
-        <is>
-          <t>37329</t>
-        </is>
-      </c>
-      <c r="C67" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D67" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:021</t>
-        </is>
-      </c>
-      <c r="E67" s="5" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="B68" s="4" t="inlineStr">
-        <is>
-          <t>37330</t>
-        </is>
-      </c>
-      <c r="C68" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D68" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:025</t>
-        </is>
-      </c>
-      <c r="E68" s="5" t="inlineStr"/>
-    </row>
-    <row r="69">
-      <c r="B69" s="4" t="inlineStr">
-        <is>
-          <t>37331</t>
-        </is>
-      </c>
-      <c r="C69" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D69" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:017</t>
-        </is>
-      </c>
-      <c r="E69" s="5" t="inlineStr"/>
-    </row>
-    <row r="70">
-      <c r="B70" s="4" t="inlineStr">
-        <is>
-          <t>37332</t>
-        </is>
-      </c>
-      <c r="C70" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D70" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:020</t>
-        </is>
-      </c>
-      <c r="E70" s="5" t="inlineStr"/>
-    </row>
-    <row r="71">
-      <c r="B71" s="4" t="inlineStr">
-        <is>
-          <t>37335</t>
-        </is>
-      </c>
-      <c r="C71" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D71" s="5" t="inlineStr">
-        <is>
-          <t>00:00:02:414</t>
-        </is>
-      </c>
-      <c r="E71" s="5" t="inlineStr"/>
-    </row>
-    <row r="72">
-      <c r="B72" s="4" t="inlineStr">
-        <is>
-          <t>37358</t>
-        </is>
-      </c>
-      <c r="C72" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D72" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:082</t>
-        </is>
-      </c>
-      <c r="E72" s="5" t="inlineStr"/>
-    </row>
-    <row r="73">
-      <c r="B73" s="4" t="inlineStr">
-        <is>
-          <t>37361</t>
-        </is>
-      </c>
-      <c r="C73" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D73" s="5" t="inlineStr">
-        <is>
-          <t>00:00:01:171</t>
-        </is>
-      </c>
-      <c r="E73" s="5" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="B74" s="4" t="inlineStr">
-        <is>
-          <t>37365</t>
-        </is>
-      </c>
-      <c r="C74" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D74" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:030</t>
-        </is>
-      </c>
-      <c r="E74" s="5" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="B75" s="4" t="inlineStr">
-        <is>
-          <t>37366</t>
-        </is>
-      </c>
-      <c r="C75" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D75" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:021</t>
-        </is>
-      </c>
-      <c r="E75" s="5" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="B76" s="4" t="inlineStr">
-        <is>
-          <t>37384</t>
-        </is>
-      </c>
-      <c r="C76" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D76" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:092</t>
-        </is>
-      </c>
-      <c r="E76" s="5" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="B77" s="4" t="inlineStr">
-        <is>
-          <t>37385</t>
-        </is>
-      </c>
-      <c r="C77" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D77" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:102</t>
-        </is>
-      </c>
-      <c r="E77" s="5" t="inlineStr"/>
-    </row>
-    <row r="78">
-      <c r="B78" s="4" t="inlineStr">
-        <is>
-          <t>37402</t>
-        </is>
-      </c>
-      <c r="C78" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D78" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:604</t>
-        </is>
-      </c>
-      <c r="E78" s="5" t="inlineStr"/>
-    </row>
-    <row r="79">
-      <c r="B79" s="4" t="inlineStr">
-        <is>
-          <t>37404</t>
-        </is>
-      </c>
-      <c r="C79" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D79" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:106</t>
-        </is>
-      </c>
-      <c r="E79" s="5" t="inlineStr"/>
-    </row>
-    <row r="80">
-      <c r="B80" s="4" t="inlineStr">
-        <is>
-          <t>37415</t>
-        </is>
-      </c>
-      <c r="C80" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D80" s="5" t="inlineStr">
-        <is>
-          <t>00:00:08:127</t>
-        </is>
-      </c>
-      <c r="E80" s="5" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="B81" s="4" t="inlineStr">
-        <is>
-          <t>37416</t>
-        </is>
-      </c>
-      <c r="C81" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D81" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:204</t>
-        </is>
-      </c>
-      <c r="E81" s="5" t="inlineStr"/>
-    </row>
-    <row r="82">
-      <c r="B82" s="4" t="inlineStr">
-        <is>
-          <t>37506</t>
-        </is>
-      </c>
-      <c r="C82" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D82" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:014</t>
-        </is>
-      </c>
-      <c r="E82" s="5" t="inlineStr"/>
-    </row>
-    <row r="83">
-      <c r="B83" s="4" t="inlineStr">
-        <is>
-          <t>37568</t>
-        </is>
-      </c>
-      <c r="C83" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D83" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:013</t>
-        </is>
-      </c>
-      <c r="E83" s="5" t="inlineStr"/>
-    </row>
-    <row r="84">
-      <c r="B84" s="4" t="inlineStr">
-        <is>
-          <t>37569</t>
-        </is>
-      </c>
-      <c r="C84" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D84" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:028</t>
-        </is>
-      </c>
-      <c r="E84" s="5" t="inlineStr"/>
-    </row>
-    <row r="85">
-      <c r="B85" s="4" t="inlineStr">
-        <is>
-          <t>37620</t>
-        </is>
-      </c>
-      <c r="C85" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D85" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:009</t>
-        </is>
-      </c>
-      <c r="E85" s="5" t="inlineStr"/>
-    </row>
-    <row r="86">
-      <c r="B86" s="4" t="inlineStr">
-        <is>
-          <t>37621</t>
-        </is>
-      </c>
-      <c r="C86" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D86" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:009</t>
-        </is>
-      </c>
-      <c r="E86" s="5" t="inlineStr"/>
-    </row>
-    <row r="87">
-      <c r="B87" s="4" t="inlineStr">
-        <is>
-          <t>37622</t>
-        </is>
-      </c>
-      <c r="C87" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D87" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:010</t>
-        </is>
-      </c>
-      <c r="E87" s="5" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="B88" s="4" t="inlineStr">
-        <is>
-          <t>37627</t>
-        </is>
-      </c>
-      <c r="C88" s="5" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="D88" s="5" t="inlineStr">
-        <is>
-          <t>00:00:00:009</t>
-        </is>
-      </c>
-      <c r="E88" s="5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>